<commit_message>
Add R files for extracting phylum, performing ANCOM, and building PCoAs.
</commit_message>
<xml_diff>
--- a/data/metadata.xlsx
+++ b/data/metadata.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/z_mcadams/OneDrive - University of Missouri/Projects/current/16S_side_projects/220114_WashU_Covid/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mailmissouri-my.sharepoint.com/personal/zlmg2b_umsystem_edu/Documents/Projects/current/16S_side_projects/220114_WashU_Covid/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{359BB456-5970-D849-888B-3A0B30953794}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{359BB456-5970-D849-888B-3A0B30953794}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6D113D75-F148-1240-8BDB-9463FFDF40DD}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="16440" xr2:uid="{1435C6D9-D6DD-C846-B0E5-EA9BD64192D7}"/>
   </bookViews>
@@ -1606,8 +1606,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FE9A1DE-B63C-CB4B-9A5D-69F13079304A}">
   <dimension ref="A1:AH277"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="50" workbookViewId="0">
-      <selection activeCell="AH128" sqref="AH128:AH151"/>
+    <sheetView tabSelected="1" topLeftCell="A239" zoomScale="125" workbookViewId="0">
+      <selection activeCell="A127" sqref="A2:XFD127"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1733,7 +1733,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
@@ -1837,7 +1837,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
@@ -1941,7 +1941,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>9</v>
       </c>
@@ -2045,7 +2045,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>11</v>
       </c>
@@ -2149,7 +2149,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>14</v>
       </c>
@@ -2253,7 +2253,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>16</v>
       </c>
@@ -2357,7 +2357,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>18</v>
       </c>
@@ -2461,7 +2461,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>21</v>
       </c>
@@ -2565,7 +2565,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>23</v>
       </c>
@@ -2669,7 +2669,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>25</v>
       </c>
@@ -2773,7 +2773,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>28</v>
       </c>
@@ -2877,7 +2877,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>30</v>
       </c>
@@ -2981,7 +2981,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="14" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>32</v>
       </c>
@@ -3085,7 +3085,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="15" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>35</v>
       </c>
@@ -3189,7 +3189,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="16" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>37</v>
       </c>
@@ -3293,7 +3293,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="17" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>39</v>
       </c>
@@ -3397,7 +3397,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="18" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>42</v>
       </c>
@@ -3501,7 +3501,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="19" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>44</v>
       </c>
@@ -3605,7 +3605,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="20" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
         <v>46</v>
       </c>
@@ -3709,7 +3709,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="21" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
         <v>48</v>
       </c>
@@ -3813,7 +3813,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="22" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
         <v>50</v>
       </c>
@@ -3917,7 +3917,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="23" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
         <v>52</v>
       </c>
@@ -4021,7 +4021,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="24" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
         <v>54</v>
       </c>
@@ -4125,7 +4125,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="25" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
         <v>56</v>
       </c>
@@ -4229,7 +4229,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="26" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
         <v>58</v>
       </c>
@@ -4333,7 +4333,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="27" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
         <v>60</v>
       </c>
@@ -4437,7 +4437,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="28" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
         <v>62</v>
       </c>
@@ -4541,7 +4541,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="29" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
         <v>64</v>
       </c>
@@ -4645,7 +4645,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="30" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
         <v>66</v>
       </c>
@@ -4749,7 +4749,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="31" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
         <v>68</v>
       </c>
@@ -4853,7 +4853,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="32" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
         <v>70</v>
       </c>
@@ -4957,7 +4957,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="33" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
         <v>72</v>
       </c>
@@ -5061,7 +5061,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="34" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
         <v>73</v>
       </c>
@@ -5165,7 +5165,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="35" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
         <v>74</v>
       </c>
@@ -5269,7 +5269,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="36" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
         <v>75</v>
       </c>
@@ -5373,7 +5373,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="37" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
         <v>76</v>
       </c>
@@ -5477,7 +5477,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="38" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
         <v>77</v>
       </c>
@@ -5581,7 +5581,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="39" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39" s="4" t="s">
         <v>78</v>
       </c>
@@ -5685,7 +5685,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="40" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
         <v>79</v>
       </c>
@@ -5789,7 +5789,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="41" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
         <v>80</v>
       </c>
@@ -5893,7 +5893,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="42" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A42" s="4" t="s">
         <v>81</v>
       </c>
@@ -5997,7 +5997,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="43" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A43" s="4" t="s">
         <v>82</v>
       </c>
@@ -6101,7 +6101,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="44" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
         <v>83</v>
       </c>
@@ -6205,7 +6205,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="45" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A45" s="4" t="s">
         <v>84</v>
       </c>
@@ -6309,7 +6309,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="46" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A46" s="4" t="s">
         <v>85</v>
       </c>
@@ -6413,7 +6413,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="47" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A47" s="4" t="s">
         <v>86</v>
       </c>
@@ -6517,7 +6517,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="48" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A48" s="4" t="s">
         <v>87</v>
       </c>
@@ -6621,7 +6621,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="49" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A49" s="4" t="s">
         <v>88</v>
       </c>
@@ -6725,7 +6725,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="50" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A50" s="4" t="s">
         <v>89</v>
       </c>
@@ -6829,7 +6829,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="51" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A51" s="4" t="s">
         <v>90</v>
       </c>
@@ -6933,7 +6933,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="52" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A52" s="4" t="s">
         <v>91</v>
       </c>
@@ -7037,7 +7037,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="53" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A53" s="4" t="s">
         <v>92</v>
       </c>
@@ -7141,7 +7141,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="54" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A54" s="4" t="s">
         <v>93</v>
       </c>
@@ -7245,7 +7245,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="55" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A55" s="4" t="s">
         <v>94</v>
       </c>
@@ -7349,7 +7349,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="56" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A56" s="4" t="s">
         <v>95</v>
       </c>
@@ -7453,7 +7453,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="57" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A57" s="4" t="s">
         <v>96</v>
       </c>
@@ -7557,7 +7557,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="58" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A58" s="4" t="s">
         <v>97</v>
       </c>
@@ -7661,7 +7661,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="59" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A59" s="4" t="s">
         <v>98</v>
       </c>
@@ -7765,7 +7765,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="60" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A60" s="4" t="s">
         <v>99</v>
       </c>
@@ -7869,7 +7869,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="61" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A61" s="4" t="s">
         <v>100</v>
       </c>
@@ -7973,7 +7973,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="62" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A62" s="4" t="s">
         <v>101</v>
       </c>
@@ -8077,7 +8077,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="63" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A63" s="4" t="s">
         <v>102</v>
       </c>
@@ -8181,7 +8181,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="64" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A64" s="4" t="s">
         <v>103</v>
       </c>
@@ -8285,7 +8285,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="65" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A65" s="4" t="s">
         <v>104</v>
       </c>
@@ -8389,7 +8389,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="66" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A66" s="4" t="s">
         <v>105</v>
       </c>
@@ -8493,7 +8493,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="67" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A67" s="4" t="s">
         <v>106</v>
       </c>
@@ -8597,7 +8597,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="68" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A68" s="4" t="s">
         <v>107</v>
       </c>
@@ -8701,7 +8701,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="69" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A69" s="4" t="s">
         <v>108</v>
       </c>
@@ -8805,7 +8805,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="70" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A70" s="4" t="s">
         <v>109</v>
       </c>
@@ -8909,7 +8909,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="71" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A71" s="4" t="s">
         <v>110</v>
       </c>
@@ -9013,7 +9013,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="72" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A72" s="4" t="s">
         <v>111</v>
       </c>
@@ -9117,7 +9117,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="73" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A73" s="4" t="s">
         <v>112</v>
       </c>
@@ -9221,7 +9221,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="74" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A74" s="4" t="s">
         <v>113</v>
       </c>
@@ -9325,7 +9325,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="75" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A75" s="4" t="s">
         <v>114</v>
       </c>
@@ -9429,7 +9429,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="76" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A76" s="4" t="s">
         <v>115</v>
       </c>
@@ -9533,7 +9533,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="77" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A77" s="4" t="s">
         <v>116</v>
       </c>
@@ -9637,7 +9637,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="78" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A78" s="4" t="s">
         <v>117</v>
       </c>
@@ -9741,7 +9741,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="79" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A79" s="4" t="s">
         <v>118</v>
       </c>
@@ -9845,7 +9845,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="80" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A80" s="4" t="s">
         <v>119</v>
       </c>
@@ -9949,7 +9949,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="81" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A81" s="4" t="s">
         <v>120</v>
       </c>
@@ -10053,7 +10053,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="82" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A82" s="4" t="s">
         <v>121</v>
       </c>
@@ -10157,7 +10157,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="83" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A83" s="4" t="s">
         <v>122</v>
       </c>
@@ -10261,7 +10261,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="84" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A84" s="4" t="s">
         <v>123</v>
       </c>
@@ -10365,7 +10365,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="85" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A85" s="4" t="s">
         <v>124</v>
       </c>
@@ -10469,7 +10469,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="86" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A86" s="4" t="s">
         <v>125</v>
       </c>
@@ -10573,7 +10573,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="87" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A87" s="4" t="s">
         <v>126</v>
       </c>
@@ -10677,7 +10677,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="88" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A88" s="4" t="s">
         <v>127</v>
       </c>
@@ -10781,7 +10781,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="89" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A89" s="4" t="s">
         <v>128</v>
       </c>
@@ -10885,7 +10885,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="90" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A90" s="4" t="s">
         <v>129</v>
       </c>
@@ -10989,7 +10989,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="91" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A91" s="4" t="s">
         <v>130</v>
       </c>
@@ -11093,7 +11093,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="92" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A92" s="4" t="s">
         <v>131</v>
       </c>
@@ -11197,7 +11197,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="93" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A93" s="4" t="s">
         <v>132</v>
       </c>
@@ -11301,7 +11301,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="94" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A94" s="4" t="s">
         <v>133</v>
       </c>
@@ -11405,7 +11405,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="95" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A95" s="4" t="s">
         <v>134</v>
       </c>
@@ -11509,7 +11509,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="96" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A96" s="4" t="s">
         <v>135</v>
       </c>
@@ -11613,7 +11613,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="97" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A97" s="4" t="s">
         <v>136</v>
       </c>
@@ -11717,7 +11717,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="98" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A98" s="4" t="s">
         <v>137</v>
       </c>
@@ -11821,7 +11821,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="99" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A99" s="4" t="s">
         <v>138</v>
       </c>
@@ -11925,7 +11925,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="100" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A100" s="4" t="s">
         <v>139</v>
       </c>
@@ -12029,7 +12029,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="101" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A101" s="4" t="s">
         <v>140</v>
       </c>
@@ -12133,7 +12133,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="102" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A102" s="4" t="s">
         <v>141</v>
       </c>
@@ -12237,7 +12237,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="103" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A103" s="4" t="s">
         <v>142</v>
       </c>
@@ -12341,7 +12341,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="104" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A104" s="4" t="s">
         <v>143</v>
       </c>
@@ -12445,7 +12445,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="105" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A105" s="4" t="s">
         <v>144</v>
       </c>
@@ -12549,7 +12549,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="106" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A106" s="4" t="s">
         <v>145</v>
       </c>
@@ -12653,7 +12653,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="107" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A107" s="4" t="s">
         <v>146</v>
       </c>
@@ -12757,7 +12757,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="108" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A108" s="4" t="s">
         <v>147</v>
       </c>
@@ -12861,7 +12861,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="109" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A109" s="4" t="s">
         <v>148</v>
       </c>
@@ -12965,7 +12965,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="110" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A110" s="4" t="s">
         <v>149</v>
       </c>
@@ -13069,7 +13069,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="111" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A111" s="4" t="s">
         <v>150</v>
       </c>
@@ -13173,7 +13173,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="112" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A112" s="4" t="s">
         <v>151</v>
       </c>
@@ -13277,7 +13277,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="113" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A113" s="4" t="s">
         <v>152</v>
       </c>
@@ -13381,7 +13381,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="114" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A114" s="4" t="s">
         <v>153</v>
       </c>
@@ -13485,7 +13485,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="115" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A115" s="4" t="s">
         <v>154</v>
       </c>
@@ -13589,7 +13589,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="116" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A116" s="4" t="s">
         <v>155</v>
       </c>
@@ -13693,7 +13693,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="117" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A117" s="4" t="s">
         <v>156</v>
       </c>
@@ -13797,7 +13797,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="118" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A118" s="4" t="s">
         <v>157</v>
       </c>
@@ -13901,7 +13901,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="119" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A119" s="4" t="s">
         <v>158</v>
       </c>
@@ -14005,7 +14005,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="120" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A120" s="4" t="s">
         <v>159</v>
       </c>
@@ -14109,7 +14109,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="121" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A121" s="4" t="s">
         <v>160</v>
       </c>
@@ -14213,7 +14213,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="122" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A122" s="4" t="s">
         <v>161</v>
       </c>
@@ -14317,7 +14317,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="123" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A123" s="4" t="s">
         <v>162</v>
       </c>
@@ -14421,7 +14421,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="124" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A124" s="4" t="s">
         <v>163</v>
       </c>
@@ -14525,7 +14525,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="125" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A125" s="4" t="s">
         <v>164</v>
       </c>
@@ -14629,7 +14629,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="126" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A126" s="4" t="s">
         <v>165</v>
       </c>
@@ -14733,7 +14733,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="127" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:34" hidden="1" x14ac:dyDescent="0.2">
       <c r="A127" s="4" t="s">
         <v>166</v>
       </c>

</xml_diff>

<commit_message>
Adding R files, Q2.front analysis with only R1 reads.
</commit_message>
<xml_diff>
--- a/data/metadata.xlsx
+++ b/data/metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mailmissouri-my.sharepoint.com/personal/zlmg2b_umsystem_edu/Documents/Projects/current/16S_side_projects/220114_WashU_Covid/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{359BB456-5970-D849-888B-3A0B30953794}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6D113D75-F148-1240-8BDB-9463FFDF40DD}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{359BB456-5970-D849-888B-3A0B30953794}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{66547867-2F55-A843-8DCE-73A705E83ECF}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="16440" xr2:uid="{1435C6D9-D6DD-C846-B0E5-EA9BD64192D7}"/>
   </bookViews>
@@ -1606,7 +1606,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FE9A1DE-B63C-CB4B-9A5D-69F13079304A}">
   <dimension ref="A1:AH277"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A239" zoomScale="125" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
       <selection activeCell="A127" sqref="A2:XFD127"/>
     </sheetView>
   </sheetViews>
@@ -1617,7 +1617,8 @@
     <col min="4" max="4" width="19.5" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="10.83203125" style="1"/>
     <col min="7" max="7" width="17.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="10.83203125" style="1"/>
+    <col min="8" max="8" width="13.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="67.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12" style="1" bestFit="1" customWidth="1"/>

</xml_diff>